<commit_message>
Deploying to gh-pages from @ torstees/ncpi-fhir-ig-2@4ce979aba83cec6ea43f22991da88975687c3271 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-CommonDataModelResearchStudy.xlsx
+++ b/StructureDefinition-CommonDataModelResearchStudy.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-11-17T22:43:52+00:00</t>
+    <t>2023-11-27T20:47:53+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -389,7 +389,7 @@
     <t>extensible</t>
   </si>
   <si>
-    <t>https://nih-ncpi.github.io/ncpi-fhir-ig-2/ValueSet/study-name-type</t>
+    <t>https://nih-ncpi.github.io/ncpi-fhir-ig-2/ValueSet/study-name-type-vs</t>
   </si>
   <si>
     <t>CommonDataModelResearchStudy.description</t>
@@ -543,7 +543,7 @@
     <t>The role of the person being described.</t>
   </si>
   <si>
-    <t>https://nih-ncpi.github.io/ncpi-fhir-ig-2/ValueSet/study-personnel-role</t>
+    <t>https://nih-ncpi.github.io/ncpi-fhir-ig-2/ValueSet/study-personnel-role-vs</t>
   </si>
   <si>
     <t>CommonDataModelResearchStudy.personnel.organization</t>
@@ -880,7 +880,7 @@
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="21.57421875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="64.41015625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="67.11328125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>

</xml_diff>